<commit_message>
GAF Stundenplan löschen erfasst
</commit_message>
<xml_diff>
--- a/Doku/Stundenplan_GAFliste.xlsx
+++ b/Doku/Stundenplan_GAFliste.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>Nr.</t>
   </si>
@@ -201,6 +201,21 @@
   </si>
   <si>
     <t>Die aktuelle Planung wird auf dem Bildschirm angezeigt.</t>
+  </si>
+  <si>
+    <t>Aufruf der Funktion Stundenplan löschen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Eine Planung wurde bereits durchgeführt.
+ - Eine neue Planung soll durchgeführt werden.</t>
+  </si>
+  <si>
+    <t>1) Benutzer versucht eine neue Stundenplanberechnung durchzuführen.
+2) Eine Hinweismeldung erscheitn, dass die alte Planung zuerst gelöscht werden muss.
+3) Über den Button "Vorhandenen Plan löschen" löscht das System die bestehende Planung.</t>
+  </si>
+  <si>
+    <t>Der bestehende Stundenplan wurde aus der Datenbank entfernt.</t>
   </si>
 </sst>
 </file>
@@ -684,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -812,6 +827,31 @@
       </c>
       <c r="I4" s="8" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="135">
+      <c r="A5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>